<commit_message>
Questions can be imported from excel sheet
</commit_message>
<xml_diff>
--- a/public/questions.xlsx
+++ b/public/questions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdnas\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C854C1-32AD-45C8-A0B2-A524B0D8004A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB314E9B-57E3-481E-8148-5BBB64FB61D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{43CE33D5-0FF5-42BF-896D-4F70BA54A4A1}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>question</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>Stockhom</t>
+  </si>
+  <si>
+    <t>3,1</t>
   </si>
 </sst>
 </file>
@@ -317,6 +320,13 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="0" baseline="0"/>
+            <a:t>***Two sample rows are given.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
           <a:endParaRPr lang="en-US" sz="1400" b="1" baseline="0"/>
         </a:p>
         <a:p>
@@ -647,7 +657,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -706,8 +716,8 @@
       <c r="G2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="1">
-        <v>3</v>
+      <c r="H2" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>